<commit_message>
Edit to user submitted template for Dams
</commit_message>
<xml_diff>
--- a/docs/build/html/_downloads/a8b399bd3975e2c4574d0dfcf09811b2/damstemplate4202022.xlsx
+++ b/docs/build/html/_downloads/a8b399bd3975e2c4574d0dfcf09811b2/damstemplate4202022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\data_updates\user_submitted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\Documentation\docs\source\docs_user\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074874B3-198E-4E1B-905D-B70C361E6644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123C582-3ACD-4F35-89F4-D94B0C7CDB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21950" yWindow="2110" windowWidth="29670" windowHeight="17450" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
+    <workbookView xWindow="19640" yWindow="150" windowWidth="31980" windowHeight="19500" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
   </bookViews>
   <sheets>
     <sheet name="new_data" sheetId="1" r:id="rId1"/>
@@ -865,8 +865,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="N10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1067,75 +1067,87 @@
       <c r="C28" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="23">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F99" xr:uid="{5AF37559-2629-420A-98F2-B2DA443BA8C9}">
+  <dataValidations count="27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51:F99" xr:uid="{5AF37559-2629-420A-98F2-B2DA443BA8C9}">
       <formula1>INDIRECT($F$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E99" xr:uid="{1667F174-C0D1-425D-AE1E-FA0641E2ADB3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E51:E99" xr:uid="{1667F174-C0D1-425D-AE1E-FA0641E2ADB3}">
       <formula1>INDIRECT($E$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G99" xr:uid="{89498156-E0C9-4734-B941-966465F4E7B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G99" xr:uid="{89498156-E0C9-4734-B941-966465F4E7B2}">
       <formula1>INDIRECT($G$1)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51:Z99" xr:uid="{F36B32A2-2B7E-47AF-A769-545AF0847515}">
       <formula1>INDIRECT(I50)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H99" xr:uid="{4BB39194-6EB9-4960-B312-C170FAE496C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:H99" xr:uid="{4BB39194-6EB9-4960-B312-C170FAE496C3}">
       <formula1>INDIRECT($H$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I50" xr:uid="{ABAE0820-5601-4115-BB9C-31E9E6D9AF54}">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I50" xr:uid="{ABAE0820-5601-4115-BB9C-31E9E6D9AF54}">
       <formula1>INDIRECT($I$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J50" xr:uid="{DEE68547-BBAA-49EF-85A7-E3B7128EAF45}">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J50" xr:uid="{DEE68547-BBAA-49EF-85A7-E3B7128EAF45}">
       <formula1>INDIRECT($J$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K50" xr:uid="{DD26ED87-4654-488E-AE8B-EAE054004B9C}">
+    <dataValidation type="list" allowBlank="1" sqref="K2:K50" xr:uid="{DD26ED87-4654-488E-AE8B-EAE054004B9C}">
       <formula1>INDIRECT($K$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L50" xr:uid="{9BC55E85-0FA8-4843-BE1E-99586420BE8E}">
+    <dataValidation type="list" allowBlank="1" sqref="L2:L50" xr:uid="{9BC55E85-0FA8-4843-BE1E-99586420BE8E}">
       <formula1>INDIRECT($L$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M50" xr:uid="{AC179DE8-166A-48E9-99F7-5BA47AAC62BC}">
+    <dataValidation type="list" allowBlank="1" sqref="M2:M50" xr:uid="{AC179DE8-166A-48E9-99F7-5BA47AAC62BC}">
       <formula1>INDIRECT($M$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N50" xr:uid="{4D7E8F93-CE36-4DD9-A3EB-7DDE622D55C9}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N50" xr:uid="{4D7E8F93-CE36-4DD9-A3EB-7DDE622D55C9}">
       <formula1>INDIRECT($N$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O50" xr:uid="{A6D76EA0-E6E8-46F0-8FC7-566717DE4009}">
+    <dataValidation type="list" allowBlank="1" sqref="O2:O50" xr:uid="{A6D76EA0-E6E8-46F0-8FC7-566717DE4009}">
       <formula1>INDIRECT($O$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P50" xr:uid="{C3DCC9F0-E06A-410A-BC2A-BEB7F833CA9B}">
+    <dataValidation type="list" allowBlank="1" sqref="P2:P50" xr:uid="{C3DCC9F0-E06A-410A-BC2A-BEB7F833CA9B}">
       <formula1>INDIRECT($P$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q50" xr:uid="{8E920611-53C4-4E32-86C4-B20AFB087A04}">
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q50" xr:uid="{8E920611-53C4-4E32-86C4-B20AFB087A04}">
       <formula1>INDIRECT($Q$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R50" xr:uid="{BF444A8F-3692-4C22-B7D5-9AC749B4D7FE}">
+    <dataValidation type="list" allowBlank="1" sqref="R2:R50" xr:uid="{BF444A8F-3692-4C22-B7D5-9AC749B4D7FE}">
       <formula1>INDIRECT($R$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S50" xr:uid="{C1A61043-7610-49B6-9799-3875AC39BD2A}">
+    <dataValidation type="list" allowBlank="1" sqref="S2:S50" xr:uid="{C1A61043-7610-49B6-9799-3875AC39BD2A}">
       <formula1>INDIRECT($S$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T50" xr:uid="{218A845F-8394-47AF-AC54-101C807B51FC}">
+    <dataValidation type="list" allowBlank="1" sqref="T2:T50" xr:uid="{218A845F-8394-47AF-AC54-101C807B51FC}">
       <formula1>INDIRECT($T$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U50" xr:uid="{8EFA96F0-5548-45A0-A523-913170CC7959}">
+    <dataValidation type="list" allowBlank="1" sqref="U2:U50" xr:uid="{8EFA96F0-5548-45A0-A523-913170CC7959}">
       <formula1>INDIRECT($U$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V50" xr:uid="{41F7CE9D-4670-4F45-9E54-5F36F4F37FEA}">
+    <dataValidation type="list" allowBlank="1" sqref="V2:V50" xr:uid="{41F7CE9D-4670-4F45-9E54-5F36F4F37FEA}">
       <formula1>INDIRECT($V$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W50" xr:uid="{7A498021-8BA2-438B-A0FA-6076D41A1C26}">
+    <dataValidation type="list" allowBlank="1" sqref="W2:W50" xr:uid="{7A498021-8BA2-438B-A0FA-6076D41A1C26}">
       <formula1>INDIRECT($W$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X50" xr:uid="{D57F7E8B-25BF-4E92-BF75-FE37F82F0FCE}">
+    <dataValidation type="list" allowBlank="1" sqref="X2:X50" xr:uid="{D57F7E8B-25BF-4E92-BF75-FE37F82F0FCE}">
       <formula1>INDIRECT($X$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y50" xr:uid="{9E15A899-8A58-4726-B9DA-814FA8FBDF7C}">
+    <dataValidation type="list" allowBlank="1" sqref="Y2:Y50" xr:uid="{9E15A899-8A58-4726-B9DA-814FA8FBDF7C}">
       <formula1>INDIRECT($Y$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z50" xr:uid="{F41BE7BF-057E-4E3B-9E9C-C8B7AFA9DA5E}">
+    <dataValidation type="list" allowBlank="1" sqref="Z2:Z50" xr:uid="{F41BE7BF-057E-4E3B-9E9C-C8B7AFA9DA5E}">
       <formula1>INDIRECT($Z$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E50" xr:uid="{19A27413-45A8-4D3C-ABDD-44A91BA18C61}">
+      <formula1>INDIRECT($E$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:F50" xr:uid="{E51777D1-078F-43BA-B3B9-474EA7F07003}">
+      <formula1>INDIRECT($F$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G2:G50" xr:uid="{06B96DC9-60F7-419A-A173-9F661210FCE4}">
+      <formula1>INDIRECT($G$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="H2:H50" xr:uid="{C55D9A37-109A-4704-8B4A-02541C04258F}">
+      <formula1>INDIRECT($H$1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2057,18 +2069,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2091,6 +2103,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B103F181-233E-4DEC-9ADC-31149E3FC4B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2105,12 +2125,4 @@
     <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
A few small fixes to content and format
Stakeholder engagement and data sources search table.
</commit_message>
<xml_diff>
--- a/docs/build/html/_downloads/a8b399bd3975e2c4574d0dfcf09811b2/damstemplate4202022.xlsx
+++ b/docs/build/html/_downloads/a8b399bd3975e2c4574d0dfcf09811b2/damstemplate4202022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\Documentation\docs\source\docs_user\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123C582-3ACD-4F35-89F4-D94B0C7CDB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE4809-423E-4148-AEB2-D47B6356BFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19640" yWindow="150" windowWidth="31980" windowHeight="19500" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
   </bookViews>
@@ -865,8 +865,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>